<commit_message>
[SOL_253775] Actulizacion plantilla removiedo la noveda 170
</commit_message>
<xml_diff>
--- a/satt_standa/desnew/plantilla.xlsx
+++ b/satt_standa/desnew/plantilla.xlsx
@@ -9,16 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6270" tabRatio="990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8010" tabRatio="990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PLANTILLA" sheetId="1" r:id="rId1"/>
     <sheet name="CAUSAS Y ANALISIS A APLICAR" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1">'CAUSAS Y ANALISIS A APLICAR'!$A$1:$C$70</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="1">'CAUSAS Y ANALISIS A APLICAR'!$A$1:$C$70</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="1">'CAUSAS Y ANALISIS A APLICAR'!$A$1:$C$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CAUSAS Y ANALISIS A APLICAR'!$A$1:$C$69</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="1">'CAUSAS Y ANALISIS A APLICAR'!$A$1:$C$66</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="1">'CAUSAS Y ANALISIS A APLICAR'!$A$1:$C$66</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -35,7 +35,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B64" authorId="0" shapeId="0">
+    <comment ref="B61" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="153">
   <si>
     <t>NUMERO DE VIAJE</t>
   </si>
@@ -661,12 +661,6 @@
     </r>
   </si>
   <si>
-    <t>NICC / NEGLIGENCIA CONDUCTOR</t>
-  </si>
-  <si>
-    <t>Esta casusa debe de ser aplicada en el momento que le conductor va a incumplir la cita de cargue y el conductor no entrega detalles del porque el incumplimiento.</t>
-  </si>
-  <si>
     <t>NICC / INCIDENTES APP CONTRATACION</t>
   </si>
   <si>
@@ -1170,9 +1164,6 @@
     </r>
   </si>
   <si>
-    <t>NER /COMPARENDO DOCUMENTOS (hace referencia cuando se presentan inconsistencias en la documentacion)</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1280,42 +1271,6 @@
     </r>
   </si>
   <si>
-    <t>NER / INFRACCIONES AL CODIGO NACIONAL DE TRANSITO(demas comparendos)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Esta causa debe de ser aplicada cuando el transportador reporte que se encuentra detenido por infraciones al </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">codigo de transito  (hace referencia a los demas comparendos que se puedan presentar por infraccion del transportador).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">En el detalle de la informacion se debe de registrar ubicación exacta,placa del funcionario de la polca, detalles del evento.
-</t>
-    </r>
-  </si>
-  <si>
     <t>NER / VARADO BAJO IMPACTO (solucion a novedad menor de 4 horas)</t>
   </si>
   <si>
@@ -1707,112 +1662,6 @@
         <charset val="1"/>
       </rPr>
       <t>En el detalle de la información se debe indicar sitio donde se encuentra el vehículo.</t>
-    </r>
-  </si>
-  <si>
-    <t>NER /PUESTOS DE CONTROL POR ORGANISMOS DEL ESTADO</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Esta causa se debe de aplicar cuando e</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>l transportador notifique que se encuentra detenido por las autoridades competentes en carretera con el fin de realizar procedimientos establecidos por la ley (incautación de la mercancia por la DIAN).</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Para la modalidad </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Exportación</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> en caso que se </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>requiera abrir precinto</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">s se debe notificar a la persona encargada de alianza entre OET - L&amp;T </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">voz a voz en horario no establecido.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">En el detalle de la información se debe de registrar ubicación exacta, placa del </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">funcionario de la polca, detalles del evento.
-</t>
     </r>
   </si>
   <si>
@@ -2802,52 +2651,6 @@
     </r>
   </si>
   <si>
-    <t>NED / NOVEDAD EN DOCUMENTOS</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Esta causa se debe de aplicar cuando al realizar el seguimiento el Transportador notifique que en presenta</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> inconvenientes en el cliente porque la documentación (le falta una hoja, se le extravió las facturas, la documentación entregada no le llego completa </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">y demás que se asocien a esta rama).
-En el detalle de la información se debe de registrar </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>ubicación exacta, nombre del cliente, y demás información que tenga del cliente.</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">NED/ VALIDAR DIRECCION DE ENTREGA </t>
   </si>
   <si>
@@ -3103,6 +2906,9 @@
   </si>
   <si>
     <t xml:space="preserve">Esta casusa debe de ser aplicada en el momento que le conductor va a incumplir la cita de cargue porque tiene pendiente entregar una devolución </t>
+  </si>
+  <si>
+    <t>NER /COMPARENDOS EN LA VIA (hace referencia cuando se presentan inconsistencias en la documentacion)</t>
   </si>
 </sst>
 </file>
@@ -3379,27 +3185,6 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3468,6 +3253,27 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3567,7 +3373,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>5229225</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3867,7 +3673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -3883,22 +3689,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3910,1272 +3716,1204 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="10"/>
-    <col min="2" max="2" width="43.5703125" style="11"/>
-    <col min="3" max="3" width="119" style="12"/>
+    <col min="1" max="1" width="20.85546875" style="3"/>
+    <col min="2" max="2" width="43.5703125" style="4"/>
+    <col min="3" max="3" width="119" style="5"/>
     <col min="4" max="4" width="3.85546875"/>
     <col min="5" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:9" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+    </row>
+    <row r="2" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
         <v>269</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="18" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+    </row>
+    <row r="3" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
         <v>270</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="4" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
         <v>271</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="20" t="s">
+      <c r="D4" s="24"/>
+      <c r="E4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+    </row>
+    <row r="5" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
         <v>272</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="21" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="66" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+    </row>
+    <row r="6" spans="1:9" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
         <v>273</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="D6" s="24"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+    </row>
+    <row r="7" spans="1:9" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
         <v>274</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+    </row>
+    <row r="8" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
         <v>275</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="65.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+    </row>
+    <row r="9" spans="1:9" ht="66" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
         <v>276</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+    </row>
+    <row r="10" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
         <v>279</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+    </row>
+    <row r="11" spans="1:9" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
         <v>281</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+    </row>
+    <row r="12" spans="1:9" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
         <v>283</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="39.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+    </row>
+    <row r="13" spans="1:9" ht="40.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
         <v>329</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+    </row>
+    <row r="14" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
         <v>296</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
-        <v>170</v>
-      </c>
-      <c r="B15" s="16" t="s">
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+    </row>
+    <row r="15" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>360</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
-        <v>360</v>
-      </c>
-      <c r="B16" s="16" t="s">
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+    </row>
+    <row r="16" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>361</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+    </row>
+    <row r="17" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>358</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
-        <v>361</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
-        <v>358</v>
-      </c>
-      <c r="B18" s="16" t="s">
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+    </row>
+    <row r="18" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
+        <v>299</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A19" s="23">
-        <v>299</v>
-      </c>
-      <c r="B19" s="24" t="s">
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+    </row>
+    <row r="19" spans="1:9" ht="40.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <v>304</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" ht="39.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="23">
-        <v>304</v>
-      </c>
-      <c r="B20" s="24" t="s">
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+    </row>
+    <row r="20" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
+        <v>307</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A21" s="23">
-        <v>307</v>
-      </c>
-      <c r="B21" s="24" t="s">
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+    </row>
+    <row r="21" spans="1:9" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16">
+        <v>309</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="23">
-        <v>309</v>
-      </c>
-      <c r="B22" s="24" t="s">
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+    </row>
+    <row r="22" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16">
+        <v>311</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A23" s="23">
-        <v>311</v>
-      </c>
-      <c r="B23" s="24" t="s">
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+    </row>
+    <row r="23" spans="1:9" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
+        <v>315</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="23">
-        <v>315</v>
-      </c>
-      <c r="B24" s="24" t="s">
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+    </row>
+    <row r="24" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
+        <v>316</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="23">
-        <v>316</v>
-      </c>
-      <c r="B25" s="24" t="s">
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+    </row>
+    <row r="25" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="16">
+        <v>341</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23">
-        <v>341</v>
-      </c>
-      <c r="B26" s="24" t="s">
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+    </row>
+    <row r="26" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="16">
+        <v>201</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A27" s="23">
-        <v>201</v>
-      </c>
-      <c r="B27" s="24" t="s">
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+    </row>
+    <row r="27" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="16">
+        <v>327</v>
+      </c>
+      <c r="B27" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A28" s="23">
-        <v>327</v>
-      </c>
-      <c r="B28" s="24" t="s">
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+    </row>
+    <row r="28" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <v>301</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
-        <v>301</v>
-      </c>
-      <c r="B29" s="16" t="s">
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+    </row>
+    <row r="29" spans="1:9" ht="68.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
+        <v>302</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
-        <v>302</v>
-      </c>
-      <c r="B30" s="16" t="s">
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+    </row>
+    <row r="30" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="8">
+        <v>303</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
-        <v>303</v>
-      </c>
-      <c r="B31" s="16" t="s">
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+    </row>
+    <row r="31" spans="1:9" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="8">
+        <v>305</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" ht="39" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
-        <v>305</v>
-      </c>
-      <c r="B32" s="16" t="s">
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+    </row>
+    <row r="32" spans="1:9" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
+        <v>365</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+    </row>
+    <row r="33" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <v>308</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="15">
-        <v>306</v>
-      </c>
-      <c r="B33" s="16" t="s">
+      <c r="C33" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+    </row>
+    <row r="34" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
+        <v>312</v>
+      </c>
+      <c r="B34" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
-        <v>308</v>
-      </c>
-      <c r="B34" s="16" t="s">
+      <c r="C34" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+    </row>
+    <row r="35" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
+        <v>313</v>
+      </c>
+      <c r="B35" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
-        <v>310</v>
-      </c>
-      <c r="B35" s="27" t="s">
+      <c r="C35" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+    </row>
+    <row r="36" spans="1:9" ht="81.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
+        <v>314</v>
+      </c>
+      <c r="B36" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
-        <v>312</v>
-      </c>
-      <c r="B36" s="27" t="s">
+      <c r="C36" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+    </row>
+    <row r="37" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
+        <v>317</v>
+      </c>
+      <c r="B37" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
-        <v>313</v>
-      </c>
-      <c r="B37" s="28" t="s">
+      <c r="C37" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+    </row>
+    <row r="38" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="8">
+        <v>318</v>
+      </c>
+      <c r="B38" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="1:9" ht="81" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
-        <v>314</v>
-      </c>
-      <c r="B38" s="28" t="s">
+      <c r="C38" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+    </row>
+    <row r="39" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="8">
+        <v>319</v>
+      </c>
+      <c r="B39" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A39" s="15">
-        <v>317</v>
-      </c>
-      <c r="B39" s="28" t="s">
+      <c r="C39" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+    </row>
+    <row r="40" spans="1:9" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
+        <v>320</v>
+      </c>
+      <c r="B40" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="1:9" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="15">
-        <v>318</v>
-      </c>
-      <c r="B40" s="28" t="s">
+      <c r="C40" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+    </row>
+    <row r="41" spans="1:9" ht="40.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="8">
+        <v>321</v>
+      </c>
+      <c r="B41" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="1:9" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="15">
-        <v>319</v>
-      </c>
-      <c r="B41" s="28" t="s">
+      <c r="C41" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+    </row>
+    <row r="42" spans="1:9" ht="66" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="8">
+        <v>323</v>
+      </c>
+      <c r="B42" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="1:9" ht="79.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="15">
-        <v>320</v>
-      </c>
-      <c r="B42" s="28" t="s">
+      <c r="C42" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+    </row>
+    <row r="43" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="8">
+        <v>324</v>
+      </c>
+      <c r="B43" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="1:9" ht="39.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="15">
-        <v>321</v>
-      </c>
-      <c r="B43" s="28" t="s">
+      <c r="C43" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+    </row>
+    <row r="44" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="8">
+        <v>325</v>
+      </c>
+      <c r="B44" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="1:9" ht="92.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="15">
-        <v>322</v>
-      </c>
-      <c r="B44" s="28" t="s">
+      <c r="C44" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
+    </row>
+    <row r="45" spans="1:9" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="8">
+        <v>326</v>
+      </c>
+      <c r="B45" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C45" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="1:9" ht="65.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="15">
-        <v>323</v>
-      </c>
-      <c r="B45" s="28" t="s">
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="8">
+        <v>213</v>
+      </c>
+      <c r="B46" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C46" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A46" s="15">
-        <v>324</v>
-      </c>
-      <c r="B46" s="28" t="s">
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+    </row>
+    <row r="47" spans="1:9" ht="81.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="22">
+        <v>6</v>
+      </c>
+      <c r="B47" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C47" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A47" s="15">
-        <v>325</v>
-      </c>
-      <c r="B47" s="28" t="s">
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="30"/>
+    </row>
+    <row r="48" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="16">
+        <v>337</v>
+      </c>
+      <c r="B48" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C47" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="15">
-        <v>326</v>
-      </c>
-      <c r="B48" s="28" t="s">
+      <c r="C48" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+    </row>
+    <row r="49" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="16">
+        <v>298</v>
+      </c>
+      <c r="B49" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="15">
-        <v>213</v>
-      </c>
-      <c r="B49" s="28" t="s">
+      <c r="C49" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C49" s="22" t="s">
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="30"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="30"/>
+    </row>
+    <row r="50" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="16">
+        <v>300</v>
+      </c>
+      <c r="B50" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="1:9" ht="81" x14ac:dyDescent="0.25">
-      <c r="A50" s="29">
-        <v>6</v>
-      </c>
-      <c r="B50" s="28" t="s">
+      <c r="C50" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="16">
+        <v>328</v>
+      </c>
+      <c r="B51" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="23">
-        <v>337</v>
-      </c>
-      <c r="B51" s="30" t="s">
+      <c r="C51" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C51" s="25" t="s">
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+    </row>
+    <row r="52" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="16">
+        <v>359</v>
+      </c>
+      <c r="B52" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A52" s="23">
+      <c r="C52" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="30"/>
+      <c r="I52" s="30"/>
+    </row>
+    <row r="53" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="16">
+        <v>277</v>
+      </c>
+      <c r="B53" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="30"/>
+      <c r="H53" s="30"/>
+      <c r="I53" s="30"/>
+    </row>
+    <row r="54" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="16">
+        <v>278</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="30"/>
+      <c r="I54" s="30"/>
+    </row>
+    <row r="55" spans="1:9" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="16">
+        <v>280</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="30"/>
+      <c r="I55" s="30"/>
+    </row>
+    <row r="56" spans="1:9" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="16">
+        <v>282</v>
+      </c>
+      <c r="B56" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="30"/>
+      <c r="G56" s="30"/>
+      <c r="H56" s="30"/>
+      <c r="I56" s="30"/>
+    </row>
+    <row r="57" spans="1:9" ht="80.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="16">
+        <v>284</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="30"/>
+      <c r="G57" s="30"/>
+      <c r="H57" s="30"/>
+      <c r="I57" s="30"/>
+    </row>
+    <row r="58" spans="1:9" ht="81" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="16">
+        <v>285</v>
+      </c>
+      <c r="B58" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="30"/>
+      <c r="H58" s="30"/>
+      <c r="I58" s="30"/>
+    </row>
+    <row r="59" spans="1:9" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="16">
+        <v>286</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="30"/>
+      <c r="H59" s="30"/>
+      <c r="I59" s="30"/>
+    </row>
+    <row r="60" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="16">
+        <v>287</v>
+      </c>
+      <c r="B60" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="30"/>
+      <c r="G60" s="30"/>
+      <c r="H60" s="30"/>
+      <c r="I60" s="30"/>
+    </row>
+    <row r="61" spans="1:9" ht="66.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="16">
+        <v>288</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D61" s="24"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="30"/>
+      <c r="I61" s="30"/>
+    </row>
+    <row r="62" spans="1:9" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="16">
+        <v>290</v>
+      </c>
+      <c r="B62" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="30"/>
+      <c r="G62" s="30"/>
+      <c r="H62" s="30"/>
+      <c r="I62" s="30"/>
+    </row>
+    <row r="63" spans="1:9" ht="54" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="16">
+        <v>291</v>
+      </c>
+      <c r="B63" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="30"/>
+      <c r="I63" s="30"/>
+    </row>
+    <row r="64" spans="1:9" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="16">
+        <v>292</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D64" s="24"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="30"/>
+      <c r="I64" s="30"/>
+    </row>
+    <row r="65" spans="1:9" ht="40.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="16">
+        <v>294</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="30"/>
+      <c r="I65" s="30"/>
+    </row>
+    <row r="66" spans="1:9" ht="81.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="16">
+        <v>297</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D66" s="24"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="30"/>
+      <c r="G66" s="30"/>
+      <c r="H66" s="30"/>
+      <c r="I66" s="30"/>
+    </row>
+    <row r="67" spans="1:9" ht="66" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="16">
+        <v>350</v>
+      </c>
+      <c r="B67" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="40.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="16">
+        <v>349</v>
+      </c>
+      <c r="B68" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="53.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="16">
         <v>298</v>
       </c>
-      <c r="B52" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="C52" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A53" s="23">
-        <v>300</v>
-      </c>
-      <c r="B53" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C53" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="23">
-        <v>328</v>
-      </c>
-      <c r="B54" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C54" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A55" s="23">
-        <v>359</v>
-      </c>
-      <c r="B55" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C55" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-    </row>
-    <row r="56" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A56" s="23">
-        <v>277</v>
-      </c>
-      <c r="B56" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="C56" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-    </row>
-    <row r="57" spans="1:9" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A57" s="23">
-        <v>278</v>
-      </c>
-      <c r="B57" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="C57" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-    </row>
-    <row r="58" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="23">
-        <v>280</v>
-      </c>
-      <c r="B58" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="C58" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-    </row>
-    <row r="59" spans="1:9" ht="79.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="23">
-        <v>282</v>
-      </c>
-      <c r="B59" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="C59" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-    </row>
-    <row r="60" spans="1:9" ht="79.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="23">
-        <v>284</v>
-      </c>
-      <c r="B60" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="C60" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-    </row>
-    <row r="61" spans="1:9" ht="80.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="23">
-        <v>285</v>
-      </c>
-      <c r="B61" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="C61" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-    </row>
-    <row r="62" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="23">
-        <v>286</v>
-      </c>
-      <c r="B62" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="C62" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-    </row>
-    <row r="63" spans="1:9" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="23">
-        <v>287</v>
-      </c>
-      <c r="B63" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="C63" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-    </row>
-    <row r="64" spans="1:9" ht="66" x14ac:dyDescent="0.25">
-      <c r="A64" s="23">
-        <v>288</v>
-      </c>
-      <c r="B64" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="C64" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-    </row>
-    <row r="65" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="23">
-        <v>290</v>
-      </c>
-      <c r="B65" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="C65" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-    </row>
-    <row r="66" spans="1:9" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="23">
-        <v>291</v>
-      </c>
-      <c r="B66" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C66" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-    </row>
-    <row r="67" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A67" s="23">
-        <v>292</v>
-      </c>
-      <c r="B67" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="C67" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-    </row>
-    <row r="68" spans="1:9" ht="66" x14ac:dyDescent="0.25">
-      <c r="A68" s="23">
-        <v>293</v>
-      </c>
-      <c r="B68" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="C68" s="25" t="s">
+      <c r="B69" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D68" s="7"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-    </row>
-    <row r="69" spans="1:9" ht="39.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="23">
-        <v>294</v>
-      </c>
-      <c r="B69" s="30" t="s">
+      <c r="C69" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C69" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-    </row>
-    <row r="70" spans="1:9" ht="81" x14ac:dyDescent="0.25">
-      <c r="A70" s="23">
-        <v>297</v>
-      </c>
-      <c r="B70" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="C70" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-    </row>
-    <row r="71" spans="1:9" ht="65.25" x14ac:dyDescent="0.25">
-      <c r="A71" s="23">
-        <v>350</v>
-      </c>
-      <c r="B71" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="C71" s="25" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="39.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="23">
-        <v>349</v>
-      </c>
-      <c r="B72" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="C72" s="25" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="52.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="23">
-        <v>298</v>
-      </c>
-      <c r="B73" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="C73" s="25" t="s">
-        <v>158</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C70"/>
+  <autoFilter ref="A1:C69"/>
   <mergeCells count="7">
-    <mergeCell ref="D1:D70"/>
+    <mergeCell ref="D1:D66"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="F5:I5"/>
-    <mergeCell ref="E6:I70"/>
+    <mergeCell ref="E6:I66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>